<commit_message>
Updated Initial CAF Excel Download
</commit_message>
<xml_diff>
--- a/public/Excel Templates/CAF.xlsx
+++ b/public/Excel Templates/CAF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HRIS\hris_api\public\Excel Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAF265B-79DE-4E1F-BB51-9C9C22BA1DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80044FDC-6564-4A8C-8AE8-1B42991A1CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="120" windowWidth="26655" windowHeight="11385" xr2:uid="{8A66E213-2698-45A8-B21E-88CC94A2EFF7}"/>
+    <workbookView xWindow="2055" yWindow="1155" windowWidth="26655" windowHeight="11385" activeTab="2" xr2:uid="{8A66E213-2698-45A8-B21E-88CC94A2EFF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Permanent" sheetId="1" r:id="rId1"/>
@@ -576,7 +576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -630,25 +630,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -724,40 +705,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -784,10 +731,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
@@ -800,29 +743,88 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -836,40 +838,48 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -920,20 +930,71 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1324,14 +1385,14 @@
   </sheetPr>
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:H10"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J16" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="1.7109375" style="33" customWidth="1"/>
+    <col min="2" max="2" width="1.7109375" style="28" customWidth="1"/>
     <col min="3" max="3" width="8" style="2" customWidth="1"/>
     <col min="4" max="5" width="3.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="2" customWidth="1"/>
@@ -1339,59 +1400,59 @@
     <col min="8" max="8" width="9" style="2" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" style="2" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="34" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="29" customWidth="1"/>
     <col min="12" max="12" width="17.5703125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" style="35" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" style="30" customWidth="1"/>
     <col min="14" max="14" width="33.5703125" style="2" customWidth="1"/>
     <col min="15" max="15" width="13" style="2" customWidth="1"/>
     <col min="16" max="16" width="10.5703125" style="2" customWidth="1"/>
     <col min="17" max="17" width="9.85546875" style="2" customWidth="1"/>
-    <col min="18" max="18" width="10" style="21" customWidth="1"/>
+    <col min="18" max="18" width="10" style="16" customWidth="1"/>
     <col min="19" max="19" width="25.5703125" style="1" customWidth="1"/>
     <col min="20" max="20" width="10.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81"/>
-      <c r="O1" s="81"/>
-      <c r="P1" s="81"/>
-      <c r="Q1" s="81"/>
-      <c r="R1" s="81"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="81"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="81"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="74" t="s">
@@ -1402,15 +1463,15 @@
       <c r="D3" s="74"/>
       <c r="E3" s="74"/>
       <c r="F3" s="74"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
       <c r="L3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="36">
+      <c r="M3" s="31">
         <v>1</v>
       </c>
       <c r="N3" s="7" t="s">
@@ -1430,15 +1491,15 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
       <c r="L4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="37"/>
+      <c r="M4" s="32"/>
       <c r="N4" s="7" t="s">
         <v>5</v>
       </c>
@@ -1463,12 +1524,12 @@
       <c r="I5" s="74"/>
       <c r="J5" s="74"/>
       <c r="K5" s="74"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="78"/>
-      <c r="Q5" s="78"/>
-      <c r="R5" s="78"/>
-      <c r="S5" s="78"/>
-      <c r="T5" s="78"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="80"/>
+      <c r="Q5" s="80"/>
+      <c r="R5" s="80"/>
+      <c r="S5" s="80"/>
+      <c r="T5" s="80"/>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="74" t="s">
@@ -1478,12 +1539,12 @@
       <c r="C6" s="74"/>
       <c r="D6" s="74"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="85"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87"/>
       <c r="L6" s="7" t="s">
         <v>7</v>
       </c>
@@ -1502,12 +1563,12 @@
       <c r="C7" s="74"/>
       <c r="D7" s="74"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="85"/>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
       <c r="L7" s="7" t="s">
         <v>9</v>
       </c>
@@ -1540,16 +1601,16 @@
       <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:20" ht="39" thickBot="1">
-      <c r="A9" s="82" t="s">
+      <c r="A9" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="83"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="84"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="86"/>
       <c r="I9" s="11" t="s">
         <v>11</v>
       </c>
@@ -1562,10 +1623,10 @@
       <c r="L9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="82" t="s">
+      <c r="M9" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="84"/>
+      <c r="N9" s="86"/>
       <c r="O9" s="11" t="s">
         <v>16</v>
       </c>
@@ -1578,164 +1639,164 @@
       <c r="R9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="S9" s="55" t="s">
+      <c r="S9" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="T9" s="56" t="s">
+      <c r="T9" s="41" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="38">
+    <row r="10" spans="1:20" s="52" customFormat="1">
+      <c r="A10" s="44">
         <v>1</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="89"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="54"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="48"/>
       <c r="M10" s="70"/>
       <c r="N10" s="71"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="42"/>
-      <c r="S10" s="43"/>
-      <c r="T10" s="63"/>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="14"/>
-      <c r="B11" s="44">
+      <c r="O10" s="48"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="92"/>
+      <c r="S10" s="50"/>
+      <c r="T10" s="51"/>
+    </row>
+    <row r="11" spans="1:20" s="52" customFormat="1">
+      <c r="A11" s="53"/>
+      <c r="B11" s="54">
         <f>B10</f>
         <v>0</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
       <c r="F11" s="68"/>
       <c r="G11" s="68"/>
       <c r="H11" s="69"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="21"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="57"/>
       <c r="M11" s="72"/>
       <c r="N11" s="73"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="64"/>
-    </row>
-    <row r="12" spans="1:20">
-      <c r="A12" s="14"/>
-      <c r="B12" s="44">
+      <c r="O11" s="58"/>
+      <c r="P11" s="59"/>
+      <c r="Q11" s="59"/>
+      <c r="R11" s="93"/>
+      <c r="S11" s="60"/>
+      <c r="T11" s="61"/>
+    </row>
+    <row r="12" spans="1:20" s="52" customFormat="1">
+      <c r="A12" s="53"/>
+      <c r="B12" s="54">
         <f>B10</f>
         <v>0</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C12" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
       <c r="F12" s="68"/>
       <c r="G12" s="68"/>
       <c r="H12" s="69"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="21"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="57"/>
       <c r="M12" s="72"/>
       <c r="N12" s="73"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="59"/>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="14"/>
-      <c r="B13" s="44">
+      <c r="O12" s="58"/>
+      <c r="P12" s="59"/>
+      <c r="Q12" s="59"/>
+      <c r="R12" s="93"/>
+      <c r="S12" s="60"/>
+      <c r="T12" s="62"/>
+    </row>
+    <row r="13" spans="1:20" s="52" customFormat="1">
+      <c r="A13" s="53"/>
+      <c r="B13" s="54">
         <f>B10</f>
         <v>0</v>
       </c>
-      <c r="C13" s="65" t="s">
+      <c r="C13" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
       <c r="F13" s="68"/>
       <c r="G13" s="68"/>
       <c r="H13" s="69"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="21"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="57"/>
       <c r="M13" s="72"/>
       <c r="N13" s="73"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="59"/>
-    </row>
-    <row r="14" spans="1:20">
-      <c r="A14" s="14"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="69"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="21"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="59"/>
+      <c r="Q13" s="59"/>
+      <c r="R13" s="93"/>
+      <c r="S13" s="60"/>
+      <c r="T13" s="62"/>
+    </row>
+    <row r="14" spans="1:20" s="52" customFormat="1">
+      <c r="A14" s="53"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="57"/>
       <c r="M14" s="72"/>
       <c r="N14" s="73"/>
-      <c r="O14" s="46"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="59"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="59"/>
+      <c r="Q14" s="59"/>
+      <c r="R14" s="93"/>
+      <c r="S14" s="60"/>
+      <c r="T14" s="62"/>
     </row>
     <row r="15" spans="1:20" ht="16.5" thickBot="1">
-      <c r="A15" s="53"/>
-      <c r="B15" s="47">
+      <c r="A15" s="39"/>
+      <c r="B15" s="33">
         <f>B10</f>
         <v>0</v>
       </c>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="57"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="89"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="42"/>
       <c r="M15" s="66"/>
       <c r="N15" s="67"/>
-      <c r="O15" s="49"/>
-      <c r="P15" s="50"/>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="51"/>
-      <c r="S15" s="52"/>
-      <c r="T15" s="61"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="38"/>
+      <c r="T15" s="91"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="5" t="s">
@@ -1750,16 +1811,16 @@
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
-      <c r="K16" s="19"/>
+      <c r="K16" s="14"/>
       <c r="L16" s="10"/>
-      <c r="M16" s="20"/>
+      <c r="M16" s="15"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
-      <c r="Q16" s="20" t="s">
+      <c r="Q16" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="T16" s="21"/>
+      <c r="T16" s="16"/>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="5" t="s">
@@ -1769,20 +1830,20 @@
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="20"/>
+      <c r="F17" s="15"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
-      <c r="K17" s="19"/>
+      <c r="K17" s="14"/>
       <c r="L17" s="10"/>
-      <c r="M17" s="20"/>
+      <c r="M17" s="15"/>
       <c r="N17" s="5"/>
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
-      <c r="T17" s="21"/>
+      <c r="T17" s="16"/>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="5" t="s">
@@ -1792,20 +1853,20 @@
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="20"/>
+      <c r="F18" s="15"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
-      <c r="K18" s="19"/>
+      <c r="K18" s="14"/>
       <c r="L18" s="10"/>
-      <c r="M18" s="20"/>
+      <c r="M18" s="15"/>
       <c r="N18" s="5"/>
       <c r="O18" s="8"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="T18" s="21"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="T18" s="16"/>
     </row>
     <row r="19" spans="1:20" ht="16.5" thickBot="1">
       <c r="A19" s="5"/>
@@ -1813,20 +1874,20 @@
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="20"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
-      <c r="K19" s="19"/>
+      <c r="K19" s="14"/>
       <c r="L19" s="10"/>
-      <c r="M19" s="20"/>
+      <c r="M19" s="15"/>
       <c r="N19" s="5"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="T19" s="21"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="T19" s="16"/>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="5"/>
@@ -1834,22 +1895,22 @@
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="20"/>
+      <c r="F20" s="15"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
-      <c r="K20" s="19"/>
+      <c r="K20" s="14"/>
       <c r="L20" s="10"/>
-      <c r="M20" s="20"/>
+      <c r="M20" s="15"/>
       <c r="N20" s="5"/>
-      <c r="O20" s="79" t="s">
+      <c r="O20" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="P20" s="79"/>
-      <c r="Q20" s="79"/>
-      <c r="R20" s="79"/>
-      <c r="T20" s="21"/>
+      <c r="P20" s="81"/>
+      <c r="Q20" s="81"/>
+      <c r="R20" s="81"/>
+      <c r="T20" s="16"/>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" s="5"/>
@@ -1857,135 +1918,135 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="20"/>
+      <c r="F21" s="15"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
-      <c r="K21" s="19"/>
+      <c r="K21" s="14"/>
       <c r="L21" s="10"/>
-      <c r="M21" s="20"/>
+      <c r="M21" s="15"/>
       <c r="N21" s="5"/>
       <c r="O21" s="8"/>
       <c r="R21" s="2"/>
-      <c r="T21" s="21"/>
+      <c r="T21" s="16"/>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="78" t="s">
+      <c r="A22" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="78"/>
-      <c r="C22" s="78"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="78" t="s">
+      <c r="B22" s="80"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="J22" s="78"/>
-      <c r="K22" s="78"/>
-      <c r="L22" s="78"/>
-      <c r="M22" s="78" t="s">
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="80"/>
+      <c r="M22" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="N22" s="78"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-      <c r="T22" s="21"/>
+      <c r="N22" s="80"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="T22" s="16"/>
     </row>
     <row r="23" spans="1:20" ht="16.5" thickBot="1">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="77"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="77" t="s">
+      <c r="B23" s="79"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="J23" s="77"/>
-      <c r="K23" s="77"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="77" t="s">
+      <c r="J23" s="79"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="N23" s="77"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="27"/>
-      <c r="R23" s="27"/>
-      <c r="S23" s="28"/>
-      <c r="T23" s="21"/>
+      <c r="N23" s="79"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="16"/>
     </row>
     <row r="24" spans="1:20">
-      <c r="A24" s="77" t="s">
+      <c r="A24" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="77"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="77"/>
-      <c r="G24" s="77"/>
-      <c r="H24" s="77"/>
-      <c r="I24" s="77" t="s">
+      <c r="B24" s="79"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="77"/>
-      <c r="K24" s="77"/>
-      <c r="L24" s="77"/>
-      <c r="M24" s="77" t="s">
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="N24" s="77"/>
-      <c r="O24" s="79" t="s">
+      <c r="N24" s="79"/>
+      <c r="O24" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="P24" s="79"/>
-      <c r="Q24" s="79"/>
-      <c r="R24" s="79"/>
-      <c r="S24" s="28"/>
-      <c r="T24" s="21"/>
+      <c r="P24" s="81"/>
+      <c r="Q24" s="81"/>
+      <c r="R24" s="81"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="16"/>
     </row>
     <row r="25" spans="1:20">
-      <c r="A25" s="77" t="s">
+      <c r="A25" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="77"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77" t="s">
+      <c r="B25" s="79"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="79"/>
+      <c r="I25" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="J25" s="77"/>
-      <c r="K25" s="77"/>
-      <c r="L25" s="77"/>
-      <c r="M25" s="77" t="s">
+      <c r="J25" s="79"/>
+      <c r="K25" s="79"/>
+      <c r="L25" s="79"/>
+      <c r="M25" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="N25" s="77"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="25"/>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="28"/>
-      <c r="T25" s="21"/>
+      <c r="N25" s="79"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="23"/>
+      <c r="T25" s="16"/>
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="8"/>
-      <c r="B26" s="29"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -1998,18 +2059,18 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="80" t="s">
+      <c r="O26" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="P26" s="80"/>
+      <c r="P26" s="82"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="8"/>
-      <c r="S26" s="28"/>
-      <c r="T26" s="21"/>
+      <c r="S26" s="23"/>
+      <c r="T26" s="16"/>
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="8"/>
-      <c r="B27" s="29"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -2026,12 +2087,12 @@
       <c r="P27" s="10"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="8"/>
-      <c r="S27" s="28"/>
-      <c r="T27" s="21"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="16"/>
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="8"/>
-      <c r="B28" s="29"/>
+      <c r="B28" s="24"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
@@ -2048,100 +2109,100 @@
       <c r="P28" s="10"/>
       <c r="Q28" s="5"/>
       <c r="R28" s="8"/>
-      <c r="S28" s="28"/>
-      <c r="T28" s="21"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="16"/>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="78" t="s">
+      <c r="A29" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="78"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="78"/>
-      <c r="H29" s="78"/>
-      <c r="I29" s="78" t="s">
+      <c r="B29" s="80"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="80"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="80"/>
+      <c r="H29" s="80"/>
+      <c r="I29" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="J29" s="78"/>
-      <c r="K29" s="78"/>
-      <c r="L29" s="78"/>
-      <c r="M29" s="78" t="s">
+      <c r="J29" s="80"/>
+      <c r="K29" s="80"/>
+      <c r="L29" s="80"/>
+      <c r="M29" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="N29" s="78"/>
-      <c r="O29" s="78" t="s">
+      <c r="N29" s="80"/>
+      <c r="O29" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="P29" s="78"/>
-      <c r="Q29" s="78"/>
-      <c r="R29" s="78"/>
-      <c r="S29" s="28"/>
-      <c r="T29" s="21"/>
+      <c r="P29" s="80"/>
+      <c r="Q29" s="80"/>
+      <c r="R29" s="80"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="16"/>
     </row>
     <row r="30" spans="1:20" ht="18.75">
-      <c r="A30" s="77" t="s">
+      <c r="A30" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="77"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="77"/>
-      <c r="E30" s="77"/>
-      <c r="F30" s="77"/>
-      <c r="G30" s="77"/>
-      <c r="H30" s="77"/>
-      <c r="I30" s="77" t="s">
+      <c r="B30" s="79"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="J30" s="77"/>
-      <c r="K30" s="77"/>
-      <c r="L30" s="77"/>
-      <c r="M30" s="77" t="s">
+      <c r="J30" s="79"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="N30" s="77"/>
-      <c r="O30" s="77" t="s">
+      <c r="N30" s="79"/>
+      <c r="O30" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="P30" s="77"/>
-      <c r="Q30" s="77"/>
-      <c r="R30" s="77"/>
-      <c r="S30" s="28"/>
-      <c r="T30" s="21"/>
+      <c r="P30" s="79"/>
+      <c r="Q30" s="79"/>
+      <c r="R30" s="79"/>
+      <c r="S30" s="23"/>
+      <c r="T30" s="16"/>
     </row>
     <row r="31" spans="1:20">
-      <c r="A31" s="77" t="s">
+      <c r="A31" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="77"/>
-      <c r="C31" s="77"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="77"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="77" t="s">
+      <c r="B31" s="79"/>
+      <c r="C31" s="79"/>
+      <c r="D31" s="79"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
+      <c r="I31" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="J31" s="77"/>
-      <c r="K31" s="77"/>
-      <c r="L31" s="77"/>
-      <c r="M31" s="77" t="s">
+      <c r="J31" s="79"/>
+      <c r="K31" s="79"/>
+      <c r="L31" s="79"/>
+      <c r="M31" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="N31" s="77"/>
+      <c r="N31" s="79"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
       <c r="R31" s="8"/>
-      <c r="S31" s="28"/>
-      <c r="T31" s="21"/>
+      <c r="S31" s="23"/>
+      <c r="T31" s="16"/>
     </row>
     <row r="32" spans="1:20">
-      <c r="B32" s="30"/>
-      <c r="C32" s="31"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
@@ -2149,21 +2210,21 @@
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
-      <c r="K32" s="32"/>
+      <c r="K32" s="27"/>
       <c r="L32" s="8"/>
-      <c r="M32" s="20"/>
+      <c r="M32" s="15"/>
       <c r="N32" s="8"/>
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
       <c r="R32" s="8"/>
-      <c r="S32" s="28"/>
-      <c r="T32" s="21"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="16"/>
     </row>
     <row r="33" spans="1:20">
-      <c r="A33" s="31"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="31"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="26"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
@@ -2171,20 +2232,20 @@
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
-      <c r="K33" s="32"/>
+      <c r="K33" s="27"/>
       <c r="L33" s="8"/>
-      <c r="M33" s="20"/>
+      <c r="M33" s="15"/>
       <c r="N33" s="8"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
       <c r="R33" s="8"/>
-      <c r="T33" s="21"/>
+      <c r="T33" s="16"/>
     </row>
     <row r="34" spans="1:20">
-      <c r="A34" s="31"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="31"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="26"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
@@ -2192,9 +2253,9 @@
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
-      <c r="K34" s="32"/>
+      <c r="K34" s="27"/>
       <c r="L34" s="8"/>
-      <c r="M34" s="20"/>
+      <c r="M34" s="15"/>
       <c r="N34" s="8"/>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
@@ -2202,17 +2263,19 @@
       <c r="R34" s="8"/>
     </row>
     <row r="37" spans="1:20">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="26" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="59">
+  <mergeCells count="60">
+    <mergeCell ref="F7:K7"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C15:E15"/>
+    <mergeCell ref="O26:P26"/>
     <mergeCell ref="A1:R2"/>
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="M9:N9"/>
@@ -2228,10 +2291,17 @@
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="F6:K6"/>
-    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="I31:L31"/>
+    <mergeCell ref="M31:N31"/>
     <mergeCell ref="A29:H29"/>
     <mergeCell ref="I29:L29"/>
     <mergeCell ref="M29:N29"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="I30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="O30:R30"/>
     <mergeCell ref="O29:R29"/>
     <mergeCell ref="A23:H23"/>
     <mergeCell ref="I23:L23"/>
@@ -2243,14 +2313,7 @@
     <mergeCell ref="A25:H25"/>
     <mergeCell ref="I25:L25"/>
     <mergeCell ref="M25:N25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="I30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="O30:R30"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="I31:L31"/>
-    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="I10:I13"/>
     <mergeCell ref="O4:T4"/>
     <mergeCell ref="M15:N15"/>
     <mergeCell ref="C13:E13"/>
@@ -2266,20 +2329,19 @@
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F14:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="O29:R29">
-    <cfRule type="expression" dxfId="8" priority="19">
+    <cfRule type="expression" dxfId="14" priority="19">
       <formula>#REF!="ABSENT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O10:T15 A9:T9 A10:C15 I10:M15 F13:F15 A16:Q16 S16:T16 A17:T22 A23:H23 M23:T23 A24:T28 A30:N36 O30:T253 B37:N37 A38:N253">
-    <cfRule type="expression" dxfId="7" priority="17">
+  <conditionalFormatting sqref="O10:T15 A9:T9 I10:M10 A10:C15 J11:M13 F13:F15 I14:M15 A16:Q16 S16:T16 A17:T22 A23:H23 M23:T23 A24:T28 A30:N36 O30:T253 B37:N37 A38:N253">
+    <cfRule type="expression" dxfId="13" priority="17">
       <formula>$T9="ABSENT"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10:R15">
-    <cfRule type="cellIs" dxfId="6" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2294,14 +2356,14 @@
   </sheetPr>
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="1.7109375" style="33" customWidth="1"/>
+    <col min="2" max="2" width="1.7109375" style="28" customWidth="1"/>
     <col min="3" max="3" width="8" style="2" customWidth="1"/>
     <col min="4" max="5" width="3.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="2" customWidth="1"/>
@@ -2309,59 +2371,59 @@
     <col min="8" max="8" width="9" style="2" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" style="2" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="34" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="29" customWidth="1"/>
     <col min="12" max="12" width="17.5703125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" style="35" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" style="30" customWidth="1"/>
     <col min="14" max="14" width="33.5703125" style="2" customWidth="1"/>
     <col min="15" max="15" width="13" style="2" customWidth="1"/>
     <col min="16" max="16" width="10.5703125" style="2" customWidth="1"/>
     <col min="17" max="17" width="9.85546875" style="2" customWidth="1"/>
-    <col min="18" max="18" width="10" style="21" customWidth="1"/>
+    <col min="18" max="18" width="10" style="16" customWidth="1"/>
     <col min="19" max="19" width="25.5703125" style="1" customWidth="1"/>
     <col min="20" max="20" width="10.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81"/>
-      <c r="O1" s="81"/>
-      <c r="P1" s="81"/>
-      <c r="Q1" s="81"/>
-      <c r="R1" s="81"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="81"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="81"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="74" t="s">
@@ -2372,15 +2434,15 @@
       <c r="D3" s="74"/>
       <c r="E3" s="74"/>
       <c r="F3" s="74"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
       <c r="L3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="36">
+      <c r="M3" s="31">
         <v>1</v>
       </c>
       <c r="N3" s="7" t="s">
@@ -2400,15 +2462,15 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
       <c r="L4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="37"/>
+      <c r="M4" s="32"/>
       <c r="N4" s="7" t="s">
         <v>5</v>
       </c>
@@ -2433,12 +2495,12 @@
       <c r="I5" s="74"/>
       <c r="J5" s="74"/>
       <c r="K5" s="74"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="78"/>
-      <c r="Q5" s="78"/>
-      <c r="R5" s="78"/>
-      <c r="S5" s="78"/>
-      <c r="T5" s="78"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="80"/>
+      <c r="Q5" s="80"/>
+      <c r="R5" s="80"/>
+      <c r="S5" s="80"/>
+      <c r="T5" s="80"/>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="74" t="s">
@@ -2448,12 +2510,12 @@
       <c r="C6" s="74"/>
       <c r="D6" s="74"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="85"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87"/>
       <c r="L6" s="7" t="s">
         <v>7</v>
       </c>
@@ -2472,12 +2534,12 @@
       <c r="C7" s="74"/>
       <c r="D7" s="74"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="85"/>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
       <c r="L7" s="7" t="s">
         <v>9</v>
       </c>
@@ -2510,16 +2572,16 @@
       <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:20" ht="39" thickBot="1">
-      <c r="A9" s="82" t="s">
+      <c r="A9" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="83"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="84"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="86"/>
       <c r="I9" s="11" t="s">
         <v>11</v>
       </c>
@@ -2532,10 +2594,10 @@
       <c r="L9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="82" t="s">
+      <c r="M9" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="84"/>
+      <c r="N9" s="86"/>
       <c r="O9" s="11" t="s">
         <v>16</v>
       </c>
@@ -2548,164 +2610,164 @@
       <c r="R9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="S9" s="55" t="s">
+      <c r="S9" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="T9" s="56" t="s">
+      <c r="T9" s="41" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="38">
+    <row r="10" spans="1:20" s="52" customFormat="1">
+      <c r="A10" s="44">
         <v>1</v>
       </c>
-      <c r="B10" s="39"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="75"/>
       <c r="D10" s="75"/>
       <c r="E10" s="75"/>
       <c r="F10" s="75"/>
       <c r="G10" s="75"/>
       <c r="H10" s="76"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="54"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="48"/>
       <c r="M10" s="70"/>
       <c r="N10" s="71"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="42"/>
-      <c r="S10" s="43"/>
-      <c r="T10" s="63"/>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="14"/>
-      <c r="B11" s="44">
+      <c r="O10" s="48"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="92"/>
+      <c r="S10" s="50"/>
+      <c r="T10" s="51"/>
+    </row>
+    <row r="11" spans="1:20" s="52" customFormat="1">
+      <c r="A11" s="53"/>
+      <c r="B11" s="54">
         <f>B10</f>
         <v>0</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
       <c r="F11" s="68"/>
       <c r="G11" s="68"/>
       <c r="H11" s="69"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="21"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="57"/>
       <c r="M11" s="72"/>
       <c r="N11" s="73"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="64"/>
-    </row>
-    <row r="12" spans="1:20">
-      <c r="A12" s="14"/>
-      <c r="B12" s="44">
+      <c r="O11" s="58"/>
+      <c r="P11" s="59"/>
+      <c r="Q11" s="59"/>
+      <c r="R11" s="93"/>
+      <c r="S11" s="60"/>
+      <c r="T11" s="61"/>
+    </row>
+    <row r="12" spans="1:20" s="52" customFormat="1">
+      <c r="A12" s="53"/>
+      <c r="B12" s="54">
         <f>B10</f>
         <v>0</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C12" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
       <c r="F12" s="68"/>
       <c r="G12" s="68"/>
       <c r="H12" s="69"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="21"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="57"/>
       <c r="M12" s="72"/>
       <c r="N12" s="73"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="59"/>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="14"/>
-      <c r="B13" s="44">
+      <c r="O12" s="58"/>
+      <c r="P12" s="59"/>
+      <c r="Q12" s="59"/>
+      <c r="R12" s="93"/>
+      <c r="S12" s="60"/>
+      <c r="T12" s="62"/>
+    </row>
+    <row r="13" spans="1:20" s="52" customFormat="1">
+      <c r="A13" s="53"/>
+      <c r="B13" s="54">
         <f>B10</f>
         <v>0</v>
       </c>
-      <c r="C13" s="65" t="s">
+      <c r="C13" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
       <c r="F13" s="68"/>
       <c r="G13" s="68"/>
       <c r="H13" s="69"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="21"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="57"/>
       <c r="M13" s="72"/>
       <c r="N13" s="73"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="59"/>
-    </row>
-    <row r="14" spans="1:20">
-      <c r="A14" s="14"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="69"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="21"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="59"/>
+      <c r="Q13" s="59"/>
+      <c r="R13" s="93"/>
+      <c r="S13" s="60"/>
+      <c r="T13" s="62"/>
+    </row>
+    <row r="14" spans="1:20" s="52" customFormat="1">
+      <c r="A14" s="53"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="57"/>
       <c r="M14" s="72"/>
       <c r="N14" s="73"/>
-      <c r="O14" s="46"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="59"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="59"/>
+      <c r="Q14" s="59"/>
+      <c r="R14" s="93"/>
+      <c r="S14" s="60"/>
+      <c r="T14" s="62"/>
     </row>
     <row r="15" spans="1:20" ht="16.5" thickBot="1">
-      <c r="A15" s="53"/>
-      <c r="B15" s="47">
+      <c r="A15" s="39"/>
+      <c r="B15" s="33">
         <f>B10</f>
         <v>0</v>
       </c>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="57"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="89"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="42"/>
       <c r="M15" s="66"/>
       <c r="N15" s="67"/>
-      <c r="O15" s="49"/>
-      <c r="P15" s="50"/>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="51"/>
-      <c r="S15" s="52"/>
-      <c r="T15" s="61"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="38"/>
+      <c r="T15" s="91"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="5" t="s">
@@ -2720,16 +2782,16 @@
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
-      <c r="K16" s="19"/>
+      <c r="K16" s="14"/>
       <c r="L16" s="10"/>
-      <c r="M16" s="20"/>
+      <c r="M16" s="15"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
-      <c r="Q16" s="20" t="s">
+      <c r="Q16" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="T16" s="21"/>
+      <c r="T16" s="16"/>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="5" t="s">
@@ -2739,20 +2801,20 @@
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="20"/>
+      <c r="F17" s="15"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
-      <c r="K17" s="19"/>
+      <c r="K17" s="14"/>
       <c r="L17" s="10"/>
-      <c r="M17" s="20"/>
+      <c r="M17" s="15"/>
       <c r="N17" s="5"/>
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
-      <c r="T17" s="21"/>
+      <c r="T17" s="16"/>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="5" t="s">
@@ -2762,20 +2824,20 @@
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="20"/>
+      <c r="F18" s="15"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
-      <c r="K18" s="19"/>
+      <c r="K18" s="14"/>
       <c r="L18" s="10"/>
-      <c r="M18" s="20"/>
+      <c r="M18" s="15"/>
       <c r="N18" s="5"/>
       <c r="O18" s="8"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="T18" s="21"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="T18" s="16"/>
     </row>
     <row r="19" spans="1:20" ht="16.5" thickBot="1">
       <c r="A19" s="5"/>
@@ -2783,20 +2845,20 @@
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="20"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
-      <c r="K19" s="19"/>
+      <c r="K19" s="14"/>
       <c r="L19" s="10"/>
-      <c r="M19" s="20"/>
+      <c r="M19" s="15"/>
       <c r="N19" s="5"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="T19" s="21"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="T19" s="16"/>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="5"/>
@@ -2804,22 +2866,22 @@
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="20"/>
+      <c r="F20" s="15"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
-      <c r="K20" s="19"/>
+      <c r="K20" s="14"/>
       <c r="L20" s="10"/>
-      <c r="M20" s="20"/>
+      <c r="M20" s="15"/>
       <c r="N20" s="5"/>
-      <c r="O20" s="79" t="s">
+      <c r="O20" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="P20" s="79"/>
-      <c r="Q20" s="79"/>
-      <c r="R20" s="79"/>
-      <c r="T20" s="21"/>
+      <c r="P20" s="81"/>
+      <c r="Q20" s="81"/>
+      <c r="R20" s="81"/>
+      <c r="T20" s="16"/>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" s="5"/>
@@ -2827,135 +2889,135 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="20"/>
+      <c r="F21" s="15"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
-      <c r="K21" s="19"/>
+      <c r="K21" s="14"/>
       <c r="L21" s="10"/>
-      <c r="M21" s="20"/>
+      <c r="M21" s="15"/>
       <c r="N21" s="5"/>
       <c r="O21" s="8"/>
       <c r="R21" s="2"/>
-      <c r="T21" s="21"/>
+      <c r="T21" s="16"/>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="78" t="s">
+      <c r="A22" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="78"/>
-      <c r="C22" s="78"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="78" t="s">
+      <c r="B22" s="80"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="J22" s="78"/>
-      <c r="K22" s="78"/>
-      <c r="L22" s="78"/>
-      <c r="M22" s="78" t="s">
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="80"/>
+      <c r="M22" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="N22" s="78"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-      <c r="T22" s="21"/>
+      <c r="N22" s="80"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="T22" s="16"/>
     </row>
     <row r="23" spans="1:20" ht="16.5" thickBot="1">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="77"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="77" t="s">
+      <c r="B23" s="79"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="J23" s="77"/>
-      <c r="K23" s="77"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="77" t="s">
+      <c r="J23" s="79"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="N23" s="77"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="27"/>
-      <c r="R23" s="27"/>
-      <c r="S23" s="28"/>
-      <c r="T23" s="21"/>
+      <c r="N23" s="79"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="16"/>
     </row>
     <row r="24" spans="1:20">
-      <c r="A24" s="77" t="s">
+      <c r="A24" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="77"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="77"/>
-      <c r="G24" s="77"/>
-      <c r="H24" s="77"/>
-      <c r="I24" s="77" t="s">
+      <c r="B24" s="79"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="77"/>
-      <c r="K24" s="77"/>
-      <c r="L24" s="77"/>
-      <c r="M24" s="77" t="s">
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="N24" s="77"/>
-      <c r="O24" s="79" t="s">
+      <c r="N24" s="79"/>
+      <c r="O24" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="P24" s="79"/>
-      <c r="Q24" s="79"/>
-      <c r="R24" s="79"/>
-      <c r="S24" s="28"/>
-      <c r="T24" s="21"/>
+      <c r="P24" s="81"/>
+      <c r="Q24" s="81"/>
+      <c r="R24" s="81"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="16"/>
     </row>
     <row r="25" spans="1:20">
-      <c r="A25" s="77" t="s">
+      <c r="A25" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="77"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77" t="s">
+      <c r="B25" s="79"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="79"/>
+      <c r="I25" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="J25" s="77"/>
-      <c r="K25" s="77"/>
-      <c r="L25" s="77"/>
-      <c r="M25" s="77" t="s">
+      <c r="J25" s="79"/>
+      <c r="K25" s="79"/>
+      <c r="L25" s="79"/>
+      <c r="M25" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="N25" s="77"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="25"/>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="28"/>
-      <c r="T25" s="21"/>
+      <c r="N25" s="79"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="23"/>
+      <c r="T25" s="16"/>
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="8"/>
-      <c r="B26" s="29"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -2968,18 +3030,18 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="80" t="s">
+      <c r="O26" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="P26" s="80"/>
+      <c r="P26" s="82"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="8"/>
-      <c r="S26" s="28"/>
-      <c r="T26" s="21"/>
+      <c r="S26" s="23"/>
+      <c r="T26" s="16"/>
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="8"/>
-      <c r="B27" s="29"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -2996,12 +3058,12 @@
       <c r="P27" s="10"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="8"/>
-      <c r="S27" s="28"/>
-      <c r="T27" s="21"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="16"/>
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="8"/>
-      <c r="B28" s="29"/>
+      <c r="B28" s="24"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
@@ -3018,100 +3080,100 @@
       <c r="P28" s="10"/>
       <c r="Q28" s="5"/>
       <c r="R28" s="8"/>
-      <c r="S28" s="28"/>
-      <c r="T28" s="21"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="16"/>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="78" t="s">
+      <c r="A29" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="78"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="78"/>
-      <c r="H29" s="78"/>
-      <c r="I29" s="78" t="s">
+      <c r="B29" s="80"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="80"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="80"/>
+      <c r="H29" s="80"/>
+      <c r="I29" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="J29" s="78"/>
-      <c r="K29" s="78"/>
-      <c r="L29" s="78"/>
-      <c r="M29" s="78" t="s">
+      <c r="J29" s="80"/>
+      <c r="K29" s="80"/>
+      <c r="L29" s="80"/>
+      <c r="M29" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="N29" s="78"/>
-      <c r="O29" s="78" t="s">
+      <c r="N29" s="80"/>
+      <c r="O29" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="P29" s="78"/>
-      <c r="Q29" s="78"/>
-      <c r="R29" s="78"/>
-      <c r="S29" s="28"/>
-      <c r="T29" s="21"/>
+      <c r="P29" s="80"/>
+      <c r="Q29" s="80"/>
+      <c r="R29" s="80"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="16"/>
     </row>
     <row r="30" spans="1:20" ht="18.75">
-      <c r="A30" s="77" t="s">
+      <c r="A30" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="77"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="77"/>
-      <c r="E30" s="77"/>
-      <c r="F30" s="77"/>
-      <c r="G30" s="77"/>
-      <c r="H30" s="77"/>
-      <c r="I30" s="77" t="s">
+      <c r="B30" s="79"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="J30" s="77"/>
-      <c r="K30" s="77"/>
-      <c r="L30" s="77"/>
-      <c r="M30" s="77" t="s">
+      <c r="J30" s="79"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="N30" s="77"/>
-      <c r="O30" s="77" t="s">
+      <c r="N30" s="79"/>
+      <c r="O30" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="P30" s="77"/>
-      <c r="Q30" s="77"/>
-      <c r="R30" s="77"/>
-      <c r="S30" s="28"/>
-      <c r="T30" s="21"/>
+      <c r="P30" s="79"/>
+      <c r="Q30" s="79"/>
+      <c r="R30" s="79"/>
+      <c r="S30" s="23"/>
+      <c r="T30" s="16"/>
     </row>
     <row r="31" spans="1:20">
-      <c r="A31" s="77" t="s">
+      <c r="A31" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="77"/>
-      <c r="C31" s="77"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="77"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="77" t="s">
+      <c r="B31" s="79"/>
+      <c r="C31" s="79"/>
+      <c r="D31" s="79"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
+      <c r="I31" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="J31" s="77"/>
-      <c r="K31" s="77"/>
-      <c r="L31" s="77"/>
-      <c r="M31" s="77" t="s">
+      <c r="J31" s="79"/>
+      <c r="K31" s="79"/>
+      <c r="L31" s="79"/>
+      <c r="M31" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="N31" s="77"/>
+      <c r="N31" s="79"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
       <c r="R31" s="8"/>
-      <c r="S31" s="28"/>
-      <c r="T31" s="21"/>
+      <c r="S31" s="23"/>
+      <c r="T31" s="16"/>
     </row>
     <row r="32" spans="1:20">
-      <c r="B32" s="30"/>
-      <c r="C32" s="31"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
@@ -3119,21 +3181,21 @@
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
-      <c r="K32" s="32"/>
+      <c r="K32" s="27"/>
       <c r="L32" s="8"/>
-      <c r="M32" s="20"/>
+      <c r="M32" s="15"/>
       <c r="N32" s="8"/>
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
       <c r="R32" s="8"/>
-      <c r="S32" s="28"/>
-      <c r="T32" s="21"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="16"/>
     </row>
     <row r="33" spans="1:20">
-      <c r="A33" s="31"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="31"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="26"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
@@ -3141,20 +3203,20 @@
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
-      <c r="K33" s="32"/>
+      <c r="K33" s="27"/>
       <c r="L33" s="8"/>
-      <c r="M33" s="20"/>
+      <c r="M33" s="15"/>
       <c r="N33" s="8"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
       <c r="R33" s="8"/>
-      <c r="T33" s="21"/>
+      <c r="T33" s="16"/>
     </row>
     <row r="34" spans="1:20">
-      <c r="A34" s="31"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="31"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="26"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
@@ -3162,9 +3224,9 @@
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
-      <c r="K34" s="32"/>
+      <c r="K34" s="27"/>
       <c r="L34" s="8"/>
-      <c r="M34" s="20"/>
+      <c r="M34" s="15"/>
       <c r="N34" s="8"/>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
@@ -3172,12 +3234,12 @@
       <c r="R34" s="8"/>
     </row>
     <row r="37" spans="1:20">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="26" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="59">
+  <mergeCells count="60">
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="M14:N14"/>
@@ -3216,6 +3278,7 @@
     <mergeCell ref="C10:H10"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="M11:N11"/>
+    <mergeCell ref="I10:I13"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="F13:H13"/>
@@ -3243,7 +3306,7 @@
       <formula>#REF!="ABSENT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O10:T15 A9:T9 A10:C15 I10:M15 F13:F15 A16:Q16 S16:T16 A17:T22 A23:H23 M23:T23 A24:T28 A30:N36 O30:T253 B37:N37 A38:N253">
+  <conditionalFormatting sqref="O10:T15 A9:T9 I10:M10 A10:C15 J11:M13 F13:F15 I14:M15 A16:Q16 S16:T16 A17:T22 A23:H23 M23:T23 A24:T28 A30:N36 O30:T253 B37:N37 A38:N253">
     <cfRule type="expression" dxfId="4" priority="2">
       <formula>$T9="ABSENT"</formula>
     </cfRule>
@@ -3264,14 +3327,14 @@
   </sheetPr>
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="1.7109375" style="33" customWidth="1"/>
+    <col min="2" max="2" width="1.7109375" style="28" customWidth="1"/>
     <col min="3" max="3" width="8" style="2" customWidth="1"/>
     <col min="4" max="5" width="3.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="2" customWidth="1"/>
@@ -3279,59 +3342,59 @@
     <col min="8" max="8" width="9" style="2" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" style="2" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="34" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="29" customWidth="1"/>
     <col min="12" max="12" width="17.5703125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" style="35" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" style="30" customWidth="1"/>
     <col min="14" max="14" width="33.5703125" style="2" customWidth="1"/>
     <col min="15" max="15" width="13" style="2" customWidth="1"/>
     <col min="16" max="16" width="10.5703125" style="2" customWidth="1"/>
     <col min="17" max="17" width="9.85546875" style="2" customWidth="1"/>
-    <col min="18" max="18" width="10" style="21" customWidth="1"/>
+    <col min="18" max="18" width="10" style="16" customWidth="1"/>
     <col min="19" max="19" width="25.5703125" style="1" customWidth="1"/>
     <col min="20" max="20" width="10.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81"/>
-      <c r="O1" s="81"/>
-      <c r="P1" s="81"/>
-      <c r="Q1" s="81"/>
-      <c r="R1" s="81"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="81"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="81"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="74" t="s">
@@ -3342,15 +3405,15 @@
       <c r="D3" s="74"/>
       <c r="E3" s="74"/>
       <c r="F3" s="74"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
       <c r="L3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="36">
+      <c r="M3" s="31">
         <v>1</v>
       </c>
       <c r="N3" s="7" t="s">
@@ -3370,15 +3433,15 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
       <c r="L4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="37"/>
+      <c r="M4" s="32"/>
       <c r="N4" s="7" t="s">
         <v>5</v>
       </c>
@@ -3403,12 +3466,12 @@
       <c r="I5" s="74"/>
       <c r="J5" s="74"/>
       <c r="K5" s="74"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="78"/>
-      <c r="Q5" s="78"/>
-      <c r="R5" s="78"/>
-      <c r="S5" s="78"/>
-      <c r="T5" s="78"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="80"/>
+      <c r="Q5" s="80"/>
+      <c r="R5" s="80"/>
+      <c r="S5" s="80"/>
+      <c r="T5" s="80"/>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="74" t="s">
@@ -3418,12 +3481,12 @@
       <c r="C6" s="74"/>
       <c r="D6" s="74"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="85"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87"/>
       <c r="L6" s="7" t="s">
         <v>7</v>
       </c>
@@ -3442,12 +3505,12 @@
       <c r="C7" s="74"/>
       <c r="D7" s="74"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="85"/>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
       <c r="L7" s="7" t="s">
         <v>9</v>
       </c>
@@ -3480,16 +3543,16 @@
       <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:20" ht="39" thickBot="1">
-      <c r="A9" s="82" t="s">
+      <c r="A9" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="83"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="84"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="86"/>
       <c r="I9" s="11" t="s">
         <v>11</v>
       </c>
@@ -3502,10 +3565,10 @@
       <c r="L9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="82" t="s">
+      <c r="M9" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="84"/>
+      <c r="N9" s="86"/>
       <c r="O9" s="11" t="s">
         <v>16</v>
       </c>
@@ -3518,164 +3581,164 @@
       <c r="R9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="S9" s="55" t="s">
+      <c r="S9" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="T9" s="56" t="s">
+      <c r="T9" s="41" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="38">
+    <row r="10" spans="1:20" s="52" customFormat="1">
+      <c r="A10" s="44">
         <v>1</v>
       </c>
-      <c r="B10" s="39"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="75"/>
       <c r="D10" s="75"/>
       <c r="E10" s="75"/>
       <c r="F10" s="75"/>
       <c r="G10" s="75"/>
       <c r="H10" s="76"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="54"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="48"/>
       <c r="M10" s="70"/>
       <c r="N10" s="71"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="42"/>
-      <c r="S10" s="43"/>
-      <c r="T10" s="63"/>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="14"/>
-      <c r="B11" s="44">
+      <c r="O10" s="48"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="92"/>
+      <c r="S10" s="50"/>
+      <c r="T10" s="51"/>
+    </row>
+    <row r="11" spans="1:20" s="52" customFormat="1">
+      <c r="A11" s="53"/>
+      <c r="B11" s="54">
         <f>B10</f>
         <v>0</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
       <c r="F11" s="68"/>
       <c r="G11" s="68"/>
       <c r="H11" s="69"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="21"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="57"/>
       <c r="M11" s="72"/>
       <c r="N11" s="73"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="64"/>
-    </row>
-    <row r="12" spans="1:20">
-      <c r="A12" s="14"/>
-      <c r="B12" s="44">
+      <c r="O11" s="58"/>
+      <c r="P11" s="59"/>
+      <c r="Q11" s="59"/>
+      <c r="R11" s="93"/>
+      <c r="S11" s="60"/>
+      <c r="T11" s="61"/>
+    </row>
+    <row r="12" spans="1:20" s="52" customFormat="1">
+      <c r="A12" s="53"/>
+      <c r="B12" s="54">
         <f>B10</f>
         <v>0</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C12" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
       <c r="F12" s="68"/>
       <c r="G12" s="68"/>
       <c r="H12" s="69"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="21"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="57"/>
       <c r="M12" s="72"/>
       <c r="N12" s="73"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="59"/>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="14"/>
-      <c r="B13" s="44">
+      <c r="O12" s="58"/>
+      <c r="P12" s="59"/>
+      <c r="Q12" s="59"/>
+      <c r="R12" s="93"/>
+      <c r="S12" s="60"/>
+      <c r="T12" s="62"/>
+    </row>
+    <row r="13" spans="1:20" s="52" customFormat="1">
+      <c r="A13" s="53"/>
+      <c r="B13" s="54">
         <f>B10</f>
         <v>0</v>
       </c>
-      <c r="C13" s="65" t="s">
+      <c r="C13" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
       <c r="F13" s="68"/>
       <c r="G13" s="68"/>
       <c r="H13" s="69"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="21"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="57"/>
       <c r="M13" s="72"/>
       <c r="N13" s="73"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="59"/>
-    </row>
-    <row r="14" spans="1:20">
-      <c r="A14" s="14"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="69"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="21"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="59"/>
+      <c r="Q13" s="59"/>
+      <c r="R13" s="93"/>
+      <c r="S13" s="60"/>
+      <c r="T13" s="62"/>
+    </row>
+    <row r="14" spans="1:20" s="52" customFormat="1">
+      <c r="A14" s="53"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="57"/>
       <c r="M14" s="72"/>
       <c r="N14" s="73"/>
-      <c r="O14" s="46"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="59"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="59"/>
+      <c r="Q14" s="59"/>
+      <c r="R14" s="93"/>
+      <c r="S14" s="60"/>
+      <c r="T14" s="62"/>
     </row>
     <row r="15" spans="1:20" ht="16.5" thickBot="1">
-      <c r="A15" s="53"/>
-      <c r="B15" s="47">
+      <c r="A15" s="39"/>
+      <c r="B15" s="33">
         <f>B10</f>
         <v>0</v>
       </c>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="57"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="89"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="42"/>
       <c r="M15" s="66"/>
       <c r="N15" s="67"/>
-      <c r="O15" s="49"/>
-      <c r="P15" s="50"/>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="51"/>
-      <c r="S15" s="52"/>
-      <c r="T15" s="61"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="38"/>
+      <c r="T15" s="91"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="5" t="s">
@@ -3690,16 +3753,16 @@
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
-      <c r="K16" s="19"/>
+      <c r="K16" s="14"/>
       <c r="L16" s="10"/>
-      <c r="M16" s="20"/>
+      <c r="M16" s="15"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
-      <c r="Q16" s="20" t="s">
+      <c r="Q16" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="T16" s="21"/>
+      <c r="T16" s="16"/>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="5" t="s">
@@ -3709,20 +3772,20 @@
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="20"/>
+      <c r="F17" s="15"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
-      <c r="K17" s="19"/>
+      <c r="K17" s="14"/>
       <c r="L17" s="10"/>
-      <c r="M17" s="20"/>
+      <c r="M17" s="15"/>
       <c r="N17" s="5"/>
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
-      <c r="T17" s="21"/>
+      <c r="T17" s="16"/>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="5" t="s">
@@ -3732,20 +3795,20 @@
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="20"/>
+      <c r="F18" s="15"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
-      <c r="K18" s="19"/>
+      <c r="K18" s="14"/>
       <c r="L18" s="10"/>
-      <c r="M18" s="20"/>
+      <c r="M18" s="15"/>
       <c r="N18" s="5"/>
       <c r="O18" s="8"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="T18" s="21"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="T18" s="16"/>
     </row>
     <row r="19" spans="1:20" ht="16.5" thickBot="1">
       <c r="A19" s="5"/>
@@ -3753,20 +3816,20 @@
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="20"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
-      <c r="K19" s="19"/>
+      <c r="K19" s="14"/>
       <c r="L19" s="10"/>
-      <c r="M19" s="20"/>
+      <c r="M19" s="15"/>
       <c r="N19" s="5"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="T19" s="21"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="T19" s="16"/>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="5"/>
@@ -3774,22 +3837,22 @@
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="20"/>
+      <c r="F20" s="15"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
-      <c r="K20" s="19"/>
+      <c r="K20" s="14"/>
       <c r="L20" s="10"/>
-      <c r="M20" s="20"/>
+      <c r="M20" s="15"/>
       <c r="N20" s="5"/>
-      <c r="O20" s="79" t="s">
+      <c r="O20" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="P20" s="79"/>
-      <c r="Q20" s="79"/>
-      <c r="R20" s="79"/>
-      <c r="T20" s="21"/>
+      <c r="P20" s="81"/>
+      <c r="Q20" s="81"/>
+      <c r="R20" s="81"/>
+      <c r="T20" s="16"/>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" s="5"/>
@@ -3797,135 +3860,135 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="20"/>
+      <c r="F21" s="15"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
-      <c r="K21" s="19"/>
+      <c r="K21" s="14"/>
       <c r="L21" s="10"/>
-      <c r="M21" s="20"/>
+      <c r="M21" s="15"/>
       <c r="N21" s="5"/>
       <c r="O21" s="8"/>
       <c r="R21" s="2"/>
-      <c r="T21" s="21"/>
+      <c r="T21" s="16"/>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="78" t="s">
+      <c r="A22" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="78"/>
-      <c r="C22" s="78"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="78" t="s">
+      <c r="B22" s="80"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="J22" s="78"/>
-      <c r="K22" s="78"/>
-      <c r="L22" s="78"/>
-      <c r="M22" s="78" t="s">
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="80"/>
+      <c r="M22" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="N22" s="78"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-      <c r="T22" s="21"/>
+      <c r="N22" s="80"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="T22" s="16"/>
     </row>
     <row r="23" spans="1:20" ht="16.5" thickBot="1">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="77"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="77" t="s">
+      <c r="B23" s="79"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="J23" s="77"/>
-      <c r="K23" s="77"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="77" t="s">
+      <c r="J23" s="79"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="N23" s="77"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="27"/>
-      <c r="R23" s="27"/>
-      <c r="S23" s="28"/>
-      <c r="T23" s="21"/>
+      <c r="N23" s="79"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="16"/>
     </row>
     <row r="24" spans="1:20">
-      <c r="A24" s="77" t="s">
+      <c r="A24" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="77"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="77"/>
-      <c r="G24" s="77"/>
-      <c r="H24" s="77"/>
-      <c r="I24" s="77" t="s">
+      <c r="B24" s="79"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="77"/>
-      <c r="K24" s="77"/>
-      <c r="L24" s="77"/>
-      <c r="M24" s="77" t="s">
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="N24" s="77"/>
-      <c r="O24" s="79" t="s">
+      <c r="N24" s="79"/>
+      <c r="O24" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="P24" s="79"/>
-      <c r="Q24" s="79"/>
-      <c r="R24" s="79"/>
-      <c r="S24" s="28"/>
-      <c r="T24" s="21"/>
+      <c r="P24" s="81"/>
+      <c r="Q24" s="81"/>
+      <c r="R24" s="81"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="16"/>
     </row>
     <row r="25" spans="1:20">
-      <c r="A25" s="77" t="s">
+      <c r="A25" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="77"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77" t="s">
+      <c r="B25" s="79"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="79"/>
+      <c r="I25" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="J25" s="77"/>
-      <c r="K25" s="77"/>
-      <c r="L25" s="77"/>
-      <c r="M25" s="77" t="s">
+      <c r="J25" s="79"/>
+      <c r="K25" s="79"/>
+      <c r="L25" s="79"/>
+      <c r="M25" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="N25" s="77"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="25"/>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="28"/>
-      <c r="T25" s="21"/>
+      <c r="N25" s="79"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="23"/>
+      <c r="T25" s="16"/>
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="8"/>
-      <c r="B26" s="29"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -3938,18 +4001,18 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="80" t="s">
+      <c r="O26" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="P26" s="80"/>
+      <c r="P26" s="82"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="8"/>
-      <c r="S26" s="28"/>
-      <c r="T26" s="21"/>
+      <c r="S26" s="23"/>
+      <c r="T26" s="16"/>
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="8"/>
-      <c r="B27" s="29"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -3966,12 +4029,12 @@
       <c r="P27" s="10"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="8"/>
-      <c r="S27" s="28"/>
-      <c r="T27" s="21"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="16"/>
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="8"/>
-      <c r="B28" s="29"/>
+      <c r="B28" s="24"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
@@ -3988,100 +4051,100 @@
       <c r="P28" s="10"/>
       <c r="Q28" s="5"/>
       <c r="R28" s="8"/>
-      <c r="S28" s="28"/>
-      <c r="T28" s="21"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="16"/>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="78" t="s">
+      <c r="A29" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="78"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="78"/>
-      <c r="H29" s="78"/>
-      <c r="I29" s="78" t="s">
+      <c r="B29" s="80"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="80"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="80"/>
+      <c r="H29" s="80"/>
+      <c r="I29" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="J29" s="78"/>
-      <c r="K29" s="78"/>
-      <c r="L29" s="78"/>
-      <c r="M29" s="78" t="s">
+      <c r="J29" s="80"/>
+      <c r="K29" s="80"/>
+      <c r="L29" s="80"/>
+      <c r="M29" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="N29" s="78"/>
-      <c r="O29" s="78" t="s">
+      <c r="N29" s="80"/>
+      <c r="O29" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="P29" s="78"/>
-      <c r="Q29" s="78"/>
-      <c r="R29" s="78"/>
-      <c r="S29" s="28"/>
-      <c r="T29" s="21"/>
+      <c r="P29" s="80"/>
+      <c r="Q29" s="80"/>
+      <c r="R29" s="80"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="16"/>
     </row>
     <row r="30" spans="1:20" ht="18.75">
-      <c r="A30" s="77" t="s">
+      <c r="A30" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="77"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="77"/>
-      <c r="E30" s="77"/>
-      <c r="F30" s="77"/>
-      <c r="G30" s="77"/>
-      <c r="H30" s="77"/>
-      <c r="I30" s="77" t="s">
+      <c r="B30" s="79"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="J30" s="77"/>
-      <c r="K30" s="77"/>
-      <c r="L30" s="77"/>
-      <c r="M30" s="77" t="s">
+      <c r="J30" s="79"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="N30" s="77"/>
-      <c r="O30" s="77" t="s">
+      <c r="N30" s="79"/>
+      <c r="O30" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="P30" s="77"/>
-      <c r="Q30" s="77"/>
-      <c r="R30" s="77"/>
-      <c r="S30" s="28"/>
-      <c r="T30" s="21"/>
+      <c r="P30" s="79"/>
+      <c r="Q30" s="79"/>
+      <c r="R30" s="79"/>
+      <c r="S30" s="23"/>
+      <c r="T30" s="16"/>
     </row>
     <row r="31" spans="1:20">
-      <c r="A31" s="77" t="s">
+      <c r="A31" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="77"/>
-      <c r="C31" s="77"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="77"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="77" t="s">
+      <c r="B31" s="79"/>
+      <c r="C31" s="79"/>
+      <c r="D31" s="79"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
+      <c r="I31" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="J31" s="77"/>
-      <c r="K31" s="77"/>
-      <c r="L31" s="77"/>
-      <c r="M31" s="77" t="s">
+      <c r="J31" s="79"/>
+      <c r="K31" s="79"/>
+      <c r="L31" s="79"/>
+      <c r="M31" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="N31" s="77"/>
+      <c r="N31" s="79"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
       <c r="R31" s="8"/>
-      <c r="S31" s="28"/>
-      <c r="T31" s="21"/>
+      <c r="S31" s="23"/>
+      <c r="T31" s="16"/>
     </row>
     <row r="32" spans="1:20">
-      <c r="B32" s="30"/>
-      <c r="C32" s="31"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
@@ -4089,21 +4152,21 @@
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
-      <c r="K32" s="32"/>
+      <c r="K32" s="27"/>
       <c r="L32" s="8"/>
-      <c r="M32" s="20"/>
+      <c r="M32" s="15"/>
       <c r="N32" s="8"/>
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
       <c r="R32" s="8"/>
-      <c r="S32" s="28"/>
-      <c r="T32" s="21"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="16"/>
     </row>
     <row r="33" spans="1:20">
-      <c r="A33" s="31"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="31"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="26"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
@@ -4111,20 +4174,20 @@
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
-      <c r="K33" s="32"/>
+      <c r="K33" s="27"/>
       <c r="L33" s="8"/>
-      <c r="M33" s="20"/>
+      <c r="M33" s="15"/>
       <c r="N33" s="8"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
       <c r="R33" s="8"/>
-      <c r="T33" s="21"/>
+      <c r="T33" s="16"/>
     </row>
     <row r="34" spans="1:20">
-      <c r="A34" s="31"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="31"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="26"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
@@ -4132,9 +4195,9 @@
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
-      <c r="K34" s="32"/>
+      <c r="K34" s="27"/>
       <c r="L34" s="8"/>
-      <c r="M34" s="20"/>
+      <c r="M34" s="15"/>
       <c r="N34" s="8"/>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
@@ -4142,12 +4205,12 @@
       <c r="R34" s="8"/>
     </row>
     <row r="37" spans="1:20">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="26" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="59">
+  <mergeCells count="60">
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="M14:N14"/>
@@ -4186,6 +4249,7 @@
     <mergeCell ref="C10:H10"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="M11:N11"/>
+    <mergeCell ref="I10:I13"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="F13:H13"/>
@@ -4213,7 +4277,7 @@
       <formula>#REF!="ABSENT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O10:T15 A9:T9 A10:C15 I10:M15 F13:F15 A16:Q16 S16:T16 A17:T22 A23:H23 M23:T23 A24:T28 A30:N36 O30:T253 B37:N37 A38:N253">
+  <conditionalFormatting sqref="O10:T15 A9:T9 I10:M10 A10:C15 J11:M13 F13:F15 I14:M15 A16:Q16 S16:T16 A17:T22 A23:H23 M23:T23 A24:T28 A30:N36 O30:T253 B37:N37 A38:N253">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>$T9="ABSENT"</formula>
     </cfRule>

</xml_diff>